<commit_message>
actualizacion de la documentacion e indicadores
</commit_message>
<xml_diff>
--- a/Documentos/Planilla e Indicadores de Riesgos (6+1 Software).xlsx
+++ b/Documentos/Planilla e Indicadores de Riesgos (6+1 Software).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F38B2C-E32F-4A94-BE73-54943BF75FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AB20A1-8647-4381-A5E3-EC386A8A69A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="18192" windowHeight="9852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="4" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -454,6 +454,9 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44625766-6AE4-42B6-9CAA-C5106F528191}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1917,7 @@
       </c>
       <c r="M4" s="12">
         <f t="shared" ref="M4:M13" ca="1" si="0">TODAY()</f>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
@@ -1962,10 +1965,10 @@
       </c>
       <c r="M5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -2010,10 +2013,10 @@
       </c>
       <c r="M6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2058,7 +2061,7 @@
       </c>
       <c r="M7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
@@ -2106,7 +2109,7 @@
       </c>
       <c r="M8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
@@ -2154,10 +2157,10 @@
       </c>
       <c r="M9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2202,7 +2205,7 @@
       </c>
       <c r="M10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
@@ -2250,7 +2253,7 @@
       </c>
       <c r="M11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
@@ -2298,10 +2301,10 @@
       </c>
       <c r="M12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2346,7 +2349,7 @@
       </c>
       <c r="M13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2677,6 +2680,12 @@
       <c r="E37" s="3">
         <f t="shared" si="2"/>
         <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="16">
+        <f>SUM(E19:E37)</f>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de la documentacion RF4
</commit_message>
<xml_diff>
--- a/Documentos/Planilla e Indicadores de Riesgos (6+1 Software).xlsx
+++ b/Documentos/Planilla e Indicadores de Riesgos (6+1 Software).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3ADD2E-F4A3-4A41-B6DA-8CD14AE81EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950A4EC4-AA31-4530-A5AD-73A1ED103BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Riesgos" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Riesgos!$C$18:$E$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Riesgos!$B$32:$E$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="119">
   <si>
     <t>Riesgo</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Modelo de entrenamiento del reconocimiento facial defectuoso</t>
   </si>
   <si>
-    <t>Baja performance de la aplicación</t>
-  </si>
-  <si>
     <t>Vulnerabilidad de los datos</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
   </si>
   <si>
     <t>Listado de riesgos detectados</t>
-  </si>
-  <si>
-    <t>TOP 10 RIESGOS</t>
   </si>
   <si>
     <t>Que avise con antelacion para reasignar sus responsabilidaes</t>
@@ -284,6 +278,126 @@
   </si>
   <si>
     <t>Cerrado</t>
+  </si>
+  <si>
+    <t>No tener el hardware para realizar una buena verificación del software</t>
+  </si>
+  <si>
+    <t>TOTAL DE EXPOSICION AL RIESGO</t>
+  </si>
+  <si>
+    <t>Malas estimaciones de tiempo para las tareas</t>
+  </si>
+  <si>
+    <t>El sistema falla en la dispositivo del cliente</t>
+  </si>
+  <si>
+    <t>El sistema falla durante la presentacion ante el jurado</t>
+  </si>
+  <si>
+    <t>Problemas de rendimiento con el dispositivo</t>
+  </si>
+  <si>
+    <t>Problemas de seguridad con el sistema</t>
+  </si>
+  <si>
+    <t>Problemas de rendimiento con el sistema</t>
+  </si>
+  <si>
+    <t>El sistema no es aceptado por el alto costo de mantenimiento requerido</t>
+  </si>
+  <si>
+    <t>Se excedio en el presupuesto establecido para el proyecto</t>
+  </si>
+  <si>
+    <t>Miembros del equipo tienen problemas personales entre ellos</t>
+  </si>
+  <si>
+    <t>Dependencia excesiva de un solo miembro del equipo</t>
+  </si>
+  <si>
+    <t>Falta de experiencia sobre el gestionamiento de un proyecto</t>
+  </si>
+  <si>
+    <t>Errores en el código que generan fallos críticos en la aplicación</t>
+  </si>
+  <si>
+    <t>Probar el sistema en el lugar donde se hara la presentacion del sistema</t>
+  </si>
+  <si>
+    <t>Usar el ingenio para salvar la situacion asumiendo el fallo como algo planeado</t>
+  </si>
+  <si>
+    <t>TOP 20 RIESGOS</t>
+  </si>
+  <si>
+    <t>El miembro del que se depende tanto capacite a los demas par evitar tal dependencia</t>
+  </si>
+  <si>
+    <t>Repartir tareas mas equitativamente para que no suceda tal dependencia</t>
+  </si>
+  <si>
+    <t>Capacitarse sobre como se lo gestiona correctamente a un proyecto</t>
+  </si>
+  <si>
+    <t>Revisiones constantes con un experto en el tema para realizar las correciones</t>
+  </si>
+  <si>
+    <t>El sistema falla en el dispositivo del cliente</t>
+  </si>
+  <si>
+    <t>Probar el sistema en un dispositivo similar</t>
+  </si>
+  <si>
+    <t>Repetir la prueba, y corregir el fallo lo mas pronto posible</t>
+  </si>
+  <si>
+    <t>Tener reuniones constantes con e PO para evitar que sean cambios para los cuales no estemos preparados</t>
+  </si>
+  <si>
+    <t>Tener todo bien configurado y bien particionado para evitar que sean cambios que afecten tanto al sistema</t>
+  </si>
+  <si>
+    <t>Plantear el uso de otros medios de autenticacion fuera de la conexion a internet</t>
+  </si>
+  <si>
+    <t>Pedir mas tiempo para realizar esa funcionalidad offline la cual seria critica</t>
+  </si>
+  <si>
+    <t>Optimizar todos los sistemas de la aplicacion para evitar esos problemas de rendimiento</t>
+  </si>
+  <si>
+    <t>Realizar cambios en los algoritmos usados en el sistema para que el rendimiento sea mejor</t>
+  </si>
+  <si>
+    <t>Fomentar la buena relacion entre los miembros del equipo por medio de actividades grupales</t>
+  </si>
+  <si>
+    <t>Mantener esos conflictos por fuera de lo referente a la realizacion del proyecto</t>
+  </si>
+  <si>
+    <t>Investigar sobre el ambiente que usaremos para evitar tales problemas</t>
+  </si>
+  <si>
+    <t>Dedicar mas tiempo del requerido para solucionar esos problemas del ambiente</t>
+  </si>
+  <si>
+    <t>Realizar una candelarizacion acorde a lo que el equipo puede realizar</t>
+  </si>
+  <si>
+    <t>Solicitar mas tiempo para la realizacion de las tareas que se adeudaron</t>
+  </si>
+  <si>
+    <t>Estado
+Riesgo SP4</t>
+  </si>
+  <si>
+    <t>Impacto 
+Potencial
+Reducido SP4</t>
+  </si>
+  <si>
+    <t>Indice de Mitigacion SP4</t>
   </si>
 </sst>
 </file>
@@ -353,7 +467,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +501,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,21 +631,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -582,7 +704,65 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -858,10 +1038,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Riesgos!$E$4:$E$13</c:f>
+              <c:f>Riesgos!$E$4:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -887,9 +1067,39 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -929,39 +1139,69 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Riesgos!$J$4:$J$13</c:f>
+              <c:f>Riesgos!$J$4:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,7 +1216,17 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Impacto Potencial Reducido SP2</c:v>
+            <c:strRef>
+              <c:f>Riesgos!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Impacto 
+Potencial
+Reducido SP2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -990,39 +1240,69 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Riesgos!$M$4:$M$13</c:f>
+              <c:f>Riesgos!$M$4:$M$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,7 +1317,17 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Impacto potencialReducido SP3</c:v>
+            <c:strRef>
+              <c:f>Riesgos!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Impacto 
+Potencial
+Reducido SP3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1051,39 +1341,69 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Riesgos!$P$4:$P$13</c:f>
+              <c:f>Riesgos!$P$4:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,6 +1411,107 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2DAE-4C82-948E-F6BDB4402925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Riesgos!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Impacto 
+Potencial
+Reducido SP4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Riesgos!$S$4:$S$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26CC-483F-9A91-2C4CB85B31CF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1845,15 +2266,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>61792</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>23572</xdr:rowOff>
+      <xdr:colOff>1435231</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>5981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>768208</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>68022</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>729343</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1882,48 +2303,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1FD39DD0-1A15-401F-8BDF-4A8F07FF72CC}" name="Tabla5" displayName="Tabla5" ref="A3:T13" totalsRowShown="0" tableBorderDxfId="12">
-  <autoFilter ref="A3:T13" xr:uid="{1FD39DD0-1A15-401F-8BDF-4A8F07FF72CC}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1FD39DD0-1A15-401F-8BDF-4A8F07FF72CC}" name="Tabla5" displayName="Tabla5" ref="A3:W23" totalsRowShown="0" tableBorderDxfId="16">
+  <autoFilter ref="A3:W23" xr:uid="{1FD39DD0-1A15-401F-8BDF-4A8F07FF72CC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W23">
+    <sortCondition descending="1" ref="E3:E23"/>
+  </sortState>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{EF594B3F-4815-41D7-AE60-D02C86D9150B}" name="Riesgo">
       <calculatedColumnFormula>A3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A4AAA5EB-184F-4B98-A4C2-D1055F34F83B}" name="Descripción"/>
+    <tableColumn id="2" xr3:uid="{A4AAA5EB-184F-4B98-A4C2-D1055F34F83B}" name="Descripción" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{116CEED1-FB01-4F56-A4D6-0C46BB9B5961}" name="Probabilidad"/>
     <tableColumn id="4" xr3:uid="{733DB596-6750-4274-904B-371EACE03B53}" name="Severidad"/>
-    <tableColumn id="5" xr3:uid="{25849016-3D3F-4C14-BF44-43CAAE708306}" name="Impacto Potencial _x000a_Original" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{25849016-3D3F-4C14-BF44-43CAAE708306}" name="Impacto Potencial _x000a_Original" dataDxfId="15">
       <calculatedColumnFormula>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{99B47D03-3F5D-4653-BDBB-97E849665596}" name="Responsable"/>
     <tableColumn id="7" xr3:uid="{3EE5B033-EBB0-4083-ADD1-93C3788ACBC8}" name="Plan de _x000a_Contingencia"/>
     <tableColumn id="8" xr3:uid="{F45CCC48-156F-49B2-92CB-9417F5A67542}" name="Plan de Mitigación"/>
-    <tableColumn id="11" xr3:uid="{E3A71803-BDAE-46BA-B213-858899D3C1E6}" name="Estado_x000a_Plan _x000a_Mitigación" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{B36A9CB2-69CC-4BEA-A3F4-DE0BC85221B0}" name="Impacto _x000a_Potencial_x000a_Reducido SP1" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{C2A10210-5625-4FBA-A72F-7CFF6651DD35}" name="Índice _x000a_de_x000a_Mitigación SP1" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{E3A71803-BDAE-46BA-B213-858899D3C1E6}" name="Estado_x000a_Plan _x000a_Mitigación" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{B36A9CB2-69CC-4BEA-A3F4-DE0BC85221B0}" name="Impacto _x000a_Potencial_x000a_Reducido SP1" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{C2A10210-5625-4FBA-A72F-7CFF6651DD35}" name="Índice _x000a_de_x000a_Mitigación SP1" dataDxfId="12">
       <calculatedColumnFormula>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{D7793383-6213-42B1-A06D-4A037CD8D84B}" name="Estado_x000a_Riesgo SP1"/>
-    <tableColumn id="16" xr3:uid="{442643CC-95A8-4415-8502-E7AF466EA37B}" name="Impacto _x000a_Potencial_x000a_Reducido SP2" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{7C53F13A-AE58-4460-A6B9-7859CCE7D75F}" name="Indice de Mitigacion SP2" dataDxfId="6">
+    <tableColumn id="16" xr3:uid="{442643CC-95A8-4415-8502-E7AF466EA37B}" name="Impacto _x000a_Potencial_x000a_Reducido SP2" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{7C53F13A-AE58-4460-A6B9-7859CCE7D75F}" name="Indice de Mitigacion SP2" dataDxfId="10">
       <calculatedColumnFormula>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A2DEDD22-25B8-4096-B037-E8A7651128ED}" name="Estado_x000a_Riesgo SP2" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{3D6DA858-CFBB-4179-B2C4-541D6E64A14D}" name="Impacto _x000a_Potencial_x000a_Reducido SP3" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{E5D1C735-E0F2-437C-80B4-B1CF8CD435FE}" name="Indice de Mitigacion SP3" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{A2DEDD22-25B8-4096-B037-E8A7651128ED}" name="Estado_x000a_Riesgo SP2" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{3D6DA858-CFBB-4179-B2C4-541D6E64A14D}" name="Impacto _x000a_Potencial_x000a_Reducido SP3" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{E5D1C735-E0F2-437C-80B4-B1CF8CD435FE}" name="Indice de Mitigacion SP3" dataDxfId="7">
       <calculatedColumnFormula>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{EA480738-F372-4A98-8D67-CC85F4BC6577}" name="Estado_x000a_Riesgo SP3" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{01A64B68-5E26-444B-8DA8-3F715255641F}" name="Riesgo recurrente" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{AE6D539F-6E63-47B5-85B7-9EB6983F7AB2}" name="F. Revisión" dataDxfId="3">
+    <tableColumn id="19" xr3:uid="{EA480738-F372-4A98-8D67-CC85F4BC6577}" name="Estado_x000a_Riesgo SP3" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{78248D1F-B3BF-4F81-B2FB-9E82E93CA009}" name="Impacto _x000a_Potencial_x000a_Reducido SP4" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{5FA44A59-B29A-4EF8-8D87-1A18D2710588}" name="Indice de Mitigacion SP4" dataDxfId="0">
+      <calculatedColumnFormula>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{9CF52E11-8979-4449-BAAC-11264367739B}" name="Estado_x000a_Riesgo SP4" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{01A64B68-5E26-444B-8DA8-3F715255641F}" name="Riesgo recurrente" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{AE6D539F-6E63-47B5-85B7-9EB6983F7AB2}" name="F. Revisión" dataDxfId="4">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2129,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44625766-6AE4-42B6-9CAA-C5106F528191}">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2147,12 +2579,13 @@
     <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -2164,7 +2597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2193,45 +2626,54 @@
         <v>14</v>
       </c>
       <c r="J3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="M3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="P3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>38</v>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2247,68 +2689,80 @@
         <v>7</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="J4" s="10">
+        <v>5</v>
+      </c>
+      <c r="K4" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="10">
+        <v>5</v>
+      </c>
+      <c r="N4" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="10">
         <v>4</v>
       </c>
-      <c r="K4" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+      <c r="Q4" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
         <v>44.444444444444443</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="10">
-        <v>4</v>
-      </c>
-      <c r="N4" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="10">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>0</v>
-      </c>
       <c r="R4" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" s="12">
-        <f t="shared" ref="T4:T13" ca="1" si="0">TODAY()</f>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="S4" s="10">
+        <v>3</v>
+      </c>
+      <c r="T4" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W4" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A13" si="1">A4+1</f>
-        <v>2</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2321,39 +2775,39 @@
         <v>9</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="J5" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K5" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>22.222222222222221</v>
+        <v>44.444444444444443</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N5" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>11.111111111111111</v>
+        <v>44.444444444444443</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>10</v>
@@ -2369,23 +2823,35 @@
         <v>0</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="S5" s="10">
+        <v>0</v>
+      </c>
+      <c r="T5" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2398,71 +2864,83 @@
         <v>9</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>45</v>
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S6" s="10">
+        <v>0</v>
+      </c>
+      <c r="T6" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="K6" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>55.555555555555557</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="10">
-        <v>5</v>
-      </c>
-      <c r="N6" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>55.555555555555557</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="10">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="T6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>34</v>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2478,68 +2956,80 @@
         <v>7</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="10">
+        <v>3</v>
+      </c>
+      <c r="N7" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="10">
-        <v>1</v>
-      </c>
-      <c r="N7" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>16.666666666666664</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>16.666666666666664</v>
-      </c>
       <c r="R7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="S7" s="10">
+        <v>4</v>
+      </c>
+      <c r="T7" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W7" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -2552,39 +3042,39 @@
         <v>6</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>16.666666666666664</v>
+        <v>50</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>16.666666666666664</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>10</v>
@@ -2602,98 +3092,122 @@
       <c r="R8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="T8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="S8" s="10">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W8" s="12">
+        <f t="shared" ref="W8:W23" ca="1" si="0">TODAY()</f>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
         <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1</v>
+      </c>
+      <c r="N9" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S9" s="10">
+        <v>3</v>
+      </c>
+      <c r="T9" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
         <v>50</v>
       </c>
-      <c r="L9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="10">
-        <v>2</v>
-      </c>
-      <c r="N9" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="11">
-        <f>Tabla5[[#This Row],[Impacto 
-Potencial
-Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
-Original]]*100</f>
-        <v>16.666666666666664</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T9" s="12">
+      <c r="U9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2709,100 +3223,112 @@
         <v>7</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>50</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N10" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>50</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="P10" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>33.333333333333329</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="R10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T10" s="12">
+      <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
         <v>6</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>33.333333333333329</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>10</v>
@@ -2821,647 +3347,1732 @@
         <v>10</v>
       </c>
       <c r="P11" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>66.666666666666657</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="R11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T11" s="12">
+      <c r="S11" s="10">
+        <v>2</v>
+      </c>
+      <c r="T11" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
-        <v>4</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F12" s="10"/>
       <c r="G12" s="9" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J12" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K12" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N12" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="O12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="10">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
-        <v>50</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="R12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="T12" s="12">
+      <c r="S12" s="10">
+        <v>5</v>
+      </c>
+      <c r="T12" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
-        <v>4</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K13" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="10">
+        <v>4</v>
+      </c>
+      <c r="N13" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="10">
+        <v>4</v>
+      </c>
+      <c r="T13" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>6</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="10">
+        <v>5</v>
+      </c>
+      <c r="K14" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="10">
+        <v>3</v>
+      </c>
+      <c r="N14" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W14" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+      <c r="Y14" s="17"/>
+    </row>
+    <row r="15" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>6</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="10">
+        <v>6</v>
+      </c>
+      <c r="K15" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="10">
+        <v>6</v>
+      </c>
+      <c r="N15" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" s="10">
+        <v>5</v>
+      </c>
+      <c r="T15" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>6</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="10">
+        <v>5</v>
+      </c>
+      <c r="K16" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="10">
+        <v>4</v>
+      </c>
+      <c r="N16" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="10">
+        <v>2</v>
+      </c>
+      <c r="T16" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W16" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="10">
+        <v>6</v>
+      </c>
+      <c r="K17" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="10">
+        <v>2</v>
+      </c>
+      <c r="N17" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17" s="10">
+        <v>0</v>
+      </c>
+      <c r="T17" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V17" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W17" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="10">
+        <v>3</v>
+      </c>
+      <c r="K18" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
         <v>75</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="10">
+      <c r="L18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="10">
         <v>1</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N18" s="11">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
         <v>25</v>
       </c>
-      <c r="O13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="10">
+      <c r="O18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" s="10">
         <v>0</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q18" s="10">
         <f>Tabla5[[#This Row],[Impacto 
 Potencial
 Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
 Original]]*100</f>
         <v>0</v>
       </c>
-      <c r="R13" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="S13" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T13" s="12">
+      <c r="R18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="10">
+        <v>0</v>
+      </c>
+      <c r="T18" s="10">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="13">
-        <f>AVERAGE(C4:C13)</f>
-        <v>2.5</v>
-      </c>
-      <c r="D14" s="13">
-        <f>AVERAGE(D4:D13)</f>
-        <v>2.6</v>
-      </c>
-      <c r="E14" s="15">
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="10">
+        <v>1</v>
+      </c>
+      <c r="K19" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>25</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="10">
+        <v>1</v>
+      </c>
+      <c r="N19" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>25</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="10">
+        <v>1</v>
+      </c>
+      <c r="T19" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>25</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W19" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="10">
+        <v>4</v>
+      </c>
+      <c r="K20" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="10">
+        <v>4</v>
+      </c>
+      <c r="N20" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P20" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>75</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S20" s="10">
+        <v>2</v>
+      </c>
+      <c r="T20" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W20" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="10">
+        <v>4</v>
+      </c>
+      <c r="K21" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="10">
+        <v>2</v>
+      </c>
+      <c r="N21" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P21" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>75</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" s="10">
+        <v>1</v>
+      </c>
+      <c r="T21" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>25</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W21" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="10">
+        <v>4</v>
+      </c>
+      <c r="K22" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="10">
+        <v>4</v>
+      </c>
+      <c r="N22" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P22" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="R22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" s="10">
+        <v>2</v>
+      </c>
+      <c r="T22" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="U22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W22" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f>Tabla5[[#This Row],[Probabilidad]]*Tabla5[[#This Row],[Severidad]]</f>
+        <v>4</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="10">
+        <v>2</v>
+      </c>
+      <c r="K23" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP1]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>50</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="10">
+        <v>4</v>
+      </c>
+      <c r="N23" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP2]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP3]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>75</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23" s="10">
+        <v>5</v>
+      </c>
+      <c r="T23" s="11">
+        <f>Tabla5[[#This Row],[Impacto 
+Potencial
+Reducido SP4]]/Tabla5[[#This Row],[Impacto Potencial 
+Original]]*100</f>
+        <v>125</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W23" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="19">
+        <f>AVERAGE(C4:C23)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D24" s="19">
+        <f>AVERAGE(D4:D23)</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E24" s="14">
         <f>SUBTOTAL(109,Tabla5[Impacto Potencial 
 Original])</f>
-        <v>65</v>
-      </c>
-      <c r="J14" s="15">
+        <v>117</v>
+      </c>
+      <c r="J24" s="14">
         <f>SUBTOTAL(109,Tabla5[Impacto 
 Potencial
 Reducido SP1])</f>
+        <v>73</v>
+      </c>
+      <c r="K24" s="13">
+        <f>J24/E24*100</f>
+        <v>62.393162393162392</v>
+      </c>
+      <c r="M24" s="14">
+        <f>SUBTOTAL(109,Tabla5[Impacto 
+Potencial
+Reducido SP2])</f>
+        <v>59</v>
+      </c>
+      <c r="N24" s="16">
+        <f>M24/E24*100</f>
+        <v>50.427350427350426</v>
+      </c>
+      <c r="P24" s="14">
+        <f>SUBTOTAL(109,Tabla5[Impacto 
+Potencial
+Reducido SP3])</f>
+        <v>45</v>
+      </c>
+      <c r="Q24" s="18">
+        <f>P24/E24*100</f>
+        <v>38.461538461538467</v>
+      </c>
+      <c r="S24" s="14">
+        <f>SUBTOTAL(109,Tabla5[Impacto 
+Potencial
+Reducido SP4])</f>
+        <v>39</v>
+      </c>
+      <c r="T24" s="18">
+        <f>S24/E24*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:23" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3">
+        <f>C33*D33</f>
+        <v>9</v>
+      </c>
+      <c r="G33" s="15">
+        <f>SUM(E33:E69)</f>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3">
+        <f>C34*D34</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3</v>
+      </c>
+      <c r="D35" s="3">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3">
+        <f>C35*D35</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
+      <c r="E36" s="3">
+        <f>C36*D36</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <f>C37*D37</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3">
+        <f>C38*D38</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3">
+        <f>C39*D39</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <f>C41*D41</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3">
+        <f>C42*D42</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3">
+        <f>C43*D43</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3">
+        <f>C44*D44</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <f>C45*D45</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3">
+        <f>C46*D46</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="3">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+      <c r="E47" s="3">
+        <f>C47*D47</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3">
+        <f>C48*D48</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="3">
+        <v>2</v>
+      </c>
+      <c r="D49" s="3">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <f>C49*D49</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3">
+        <v>2</v>
+      </c>
+      <c r="E50" s="3">
+        <f>C50*D50</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>2</v>
+      </c>
+      <c r="E51" s="3">
+        <f>C51*D51</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3">
+        <f>C52*D52</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3</v>
+      </c>
+      <c r="E53" s="3">
+        <f>C53*D53</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3">
+        <f>C54*D54</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3">
+        <f>C55*D55</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <v>3</v>
+      </c>
+      <c r="E56" s="3">
+        <f>C56*D56</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3">
+        <f>C57*D57</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="3">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <v>3</v>
+      </c>
+      <c r="E58" s="3">
+        <f>C58*D58</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="14">
-        <f>J14/E14*100</f>
-        <v>40</v>
-      </c>
-      <c r="M14" s="15">
-        <f>SUBTOTAL(109,Tabla5[Impacto 
-Potencial
-Reducido SP2])</f>
-        <v>20</v>
-      </c>
-      <c r="N14" s="17">
-        <f>M14/E14*100</f>
-        <v>30.76923076923077</v>
-      </c>
-      <c r="P14" s="15">
-        <f>SUBTOTAL(109,Tabla5[Impacto 
-Potencial
-Reducido SP3])</f>
-        <v>15</v>
-      </c>
-      <c r="Q14" s="20">
-        <f>P14/E14*100</f>
-        <v>23.076923076923077</v>
-      </c>
-      <c r="U14" s="18"/>
-      <c r="V14" s="19"/>
-    </row>
-    <row r="16" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="C59" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="D59" s="3">
+        <v>3</v>
+      </c>
+      <c r="E59" s="3">
+        <f>C59*D59</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <v>3</v>
+      </c>
+      <c r="E60" s="3">
+        <f>C60*D60</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+      <c r="D61" s="3">
+        <v>3</v>
+      </c>
+      <c r="E61" s="3">
+        <f>C61*D61</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="3">
+        <v>3</v>
+      </c>
+      <c r="D62" s="3">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3">
+        <f>C62*D62</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2</v>
+      </c>
+      <c r="E63" s="3">
+        <f>C63*D63</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3">
+        <v>2</v>
+      </c>
+      <c r="E64" s="3">
+        <f>C64*D64</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C65" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3">
-        <f>C19*D19</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="D65" s="3">
+        <v>2</v>
+      </c>
+      <c r="E65" s="3">
+        <f>C65*D65</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="3">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" ref="E20:E44" si="2">C20*D20</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="D66" s="3">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3">
+        <f>C66*D66</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="3">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3">
-        <v>3</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="3">
-        <v>3</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="3">
-        <v>3</v>
-      </c>
-      <c r="D24" s="3">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="D67" s="3">
+        <v>2</v>
+      </c>
+      <c r="E67" s="3">
+        <f>C67*D67</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="3">
         <v>1</v>
       </c>
-      <c r="D25" s="3">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2</v>
-      </c>
-      <c r="D26" s="3">
-        <v>2</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2</v>
-      </c>
-      <c r="D27" s="3">
-        <v>2</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="3">
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="3">
+        <f>C68*D68</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="3">
+        <v>2</v>
+      </c>
+      <c r="D69" s="3">
         <v>1</v>
       </c>
-      <c r="D28" s="3">
-        <v>2</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29" s="3">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <v>2</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="3">
-        <v>3</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="3">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3">
-        <v>3</v>
-      </c>
-      <c r="E33" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="3">
-        <v>2</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
-      </c>
-      <c r="D35" s="3">
-        <v>2</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="3">
-        <v>3</v>
-      </c>
-      <c r="D36" s="3">
-        <v>2</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="3">
-        <v>2</v>
-      </c>
-      <c r="D37" s="3">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="3">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
-      <c r="D39" s="3">
-        <v>3</v>
-      </c>
-      <c r="E39" s="3">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <v>3</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="3">
-        <v>3</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="3">
-        <v>2</v>
-      </c>
-      <c r="D42" s="3">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="3">
-        <v>2</v>
-      </c>
-      <c r="D43" s="3">
-        <v>2</v>
-      </c>
-      <c r="E43" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="3">
-        <v>3</v>
-      </c>
-      <c r="D44" s="3">
-        <v>3</v>
-      </c>
-      <c r="E44" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="16">
-        <f>SUM(E19:E44)</f>
-        <v>117</v>
+      <c r="E69" s="3">
+        <f>C69*D69</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C18:E45" xr:uid="{44625766-6AE4-42B6-9CAA-C5106F528191}"/>
+  <autoFilter ref="B32:E32" xr:uid="{44625766-6AE4-42B6-9CAA-C5106F528191}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:E70">
+      <sortCondition descending="1" ref="E32"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C14:D14">
+  <conditionalFormatting sqref="C24:D24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3472,7 +5083,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>